<commit_message>
hoàn thành code crawl được bài đăng , bình luận, nhưng chưa lấy đưuọc bình luận con (subcomment)
</commit_message>
<xml_diff>
--- a/comment.xlsx
+++ b/comment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,7 +454,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Trúc Lâm Vũ****E tham khảo thì thấy có ng ko đốt vẫn đẻ mổ bthg có ng đốt rồi thì vẫn có bầu nhưng có ng đốt rồi thì lại khó có bầu phải đi chữa để có bầu khá là vất vả Nên e nghĩ là sẽ tuỳ cơ địa mỗi người kb trước được  Vì có ng họ phải đốt mấy lần chứ kp 1 lần C tham khảo thì nên hỏi cho kĩ</t>
+          <t>Mắt Biếc****Bạn cho mình hỏi phòng 1 người là bn tiền 1 ngày ạ</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Mk đốt xong vẫn bầu bình thường bạn chọn chỗ uy tín đốt bs chuyên là ko lo lắm đâu trc mk cũng bị độ 2 này</t>
+          <t>Lê Hà Phương****C ơi cho e hỏi chút phòng giá bn 1 ngày vậy ạ</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cát Mộng Liễu****Không ảnh hưởng j đâu em Nhưng nếu em không khó chịu j thì cứ để đẻ đi rồi chữa sau</t>
+          <t>Thùy An****Nhập viện đc là may mắn lắm ý ah</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Trúc Lâm Vũ****B bị bao lâu rồi</t>
+          <t>Nhung Le**** không nói ngoa tí nào nhưng cơm viện HN ngon thật Nhà t xui xui đã nằm đủ các viện tư thì vote cơm HN ngon nhất</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Huy Tú****Mng ai biết chỉ mình nữa với ạ</t>
+          <t xml:space="preserve">Nguyễn Lan****Nằm sướng Nhưng mỗi tội nhiều tiền e nhỉ </t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Lucky Hùng****nên đi khám đi nhé</t>
+          <t>向日葵****Cho m hỏi chút là phòng mấy nh vậy ạrộng quá</t>
         </is>
       </c>
     </row>
@@ -532,7 +532,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Huy Tú****tình trạng ntn rồi b</t>
+          <t>Hải Yến****Chu Liễu Ytam chưa có thẻ thì vô tư luôn nhé</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lucky Hùng****</t>
+          <t>Ánh Nguyệt Lê****Em chào các mom ạ Em là tư vấn tài chính bên công ty Daiichi Life Việt Nam Hiện bên em có 1 giải pháp giúp cho KH thanh toán 100 viện phí tạị tất cả các bệnh viện từ viện công đến viện tư mà không cần đúng tuyến ạ Nếu các mom quan tâm thì liên hệ 0962673255 để được tư vấn nhé ạ</t>
         </is>
       </c>
     </row>
@@ -554,11 +554,32 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Trúc Lâm Vũ****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Bảo Hiểm Dai-ichi**** Bảo Hiểm DAIICHI chi trả viện phí lên tới 1 TỶ ĐỒNG1 BỆNH
+ Bạn quan tâm bảo vệ sức khỏe Gia Đình hãy tham khảo gói BHNT Daiichi  Thẻ Chăm Sóc Sức Khỏe Tỷ suất sinh lời từ 1317năm trung bình trả 5 năm gần đây
+ Phí thẻ trẻ nhỏ rẻ chỉ từ 21 triệu năm phí rẻ nhất các công ty BHNT
+ Tien phong va an uong 3000000ngay
+ Phẫu thuật 75trca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệuca
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản KhuyếtTậtBẩm
+Sinh
+ Chi trả cho các bệnh từ nhẹ như Cảm Cúm Cúm A cho đến bệnh nghiêm trọng như Ung Thư
+ Chi trả cả các bệnh liên quan đến ThoáiHoáXương
+Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Chi trả khi nằm viện đủ 12 tiếng trở lên  rất nhiều hãng yêu cầu 24 tiếng
+ Thời gian chờ bệnh Đặc Biệt chỉ 90 ngày  nhiều hãng là 365 ngày
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần
+điều trị
+ Bảo vệ tới 75 tuổi dài hạn nhất thị trường BHNT
+ Bảo lãnh các Bệnh Viện Quốc Tế 5 VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN 108
+ Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm Mr Trọng 0987959262 Tư vấn Nhiệt Tình Tận Tâm vì Khách Hàng</t>
         </is>
       </c>
     </row>
@@ -567,11 +588,11 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Trúc Lâm Vũ****tình trạng ntn rồi b</t>
+          <t>Xuân Hoàng Bùi****Mời các mom vào đây tham khảo nhiều kiến thức chăm con bổ ích lắm Mẹ Thông Thái Nuôi Con Khoa Học</t>
         </is>
       </c>
     </row>
@@ -580,11 +601,11 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Cát Mộng Liễu****B bị bao lâu rồi</t>
+          <t>Xuân Hoàng Bùi****Mời các mom vào đây tham khảo nhiều kiến thức chăm con bổ ích lắm Mẹ Thông Thái Nuôi Con Khoa Học</t>
         </is>
       </c>
     </row>
@@ -593,11 +614,11 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Đào Mỹ Dung****Còn tí tẹo thì kệ nó thôi em Không sao đâu Về vệ sinh là được rồi</t>
+          <t>Nguyễn Bích Đào****Nó là cơ địa sẹo lồi k hết đc mom nhé Chỉ có đi thẩm mỹ mới hết thôi M mổ 2 lần con 10 tuổi rồi vẫn lồi như thường</t>
         </is>
       </c>
     </row>
@@ -606,11 +627,11 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Huy Tú****nên đi khám đi nhé</t>
+          <t>Quỳnh Như****E cũng vậy chán quá mom còn thêm quả bụg mỡ chà bá nữa sao mom giảm dk đẹp hay vậy</t>
         </is>
       </c>
     </row>
@@ -619,11 +640,11 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Huy Tú****</t>
+          <t>Hải Yến****Có thẻ BH an tâm vào nằm phòng xịn xò của HN e c nhỉ</t>
         </is>
       </c>
     </row>
@@ -632,11 +653,32 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Cát Mộng Liễu****còn tùy tình trạng tóc của b như thế nào nữa ạ</t>
+          <t>Bảo Hiểm Dai-ichi**** Bảo Hiểm DAIICHI chi trả viện phí lên tới 1 TỶ ĐỒNG1 BỆNH
+ Bạn quan tâm bảo vệ sức khỏe Gia Đình hãy tham khảo gói BHNT Daiichi  Thẻ Chăm Sóc Sức Khỏe Tỷ suất sinh lời từ 1317năm trung bình trả 5 năm gần đây
+ Phí thẻ trẻ nhỏ rẻ chỉ từ 21 triệu năm
+ Tien phong va an uong 3000000ngay
+ Phẫu thuật 75trca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệu
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản KhuyếtTậtBẩm
+Sinh
+ Chi trả cho các bệnh từ nhẹ như Cảm Cúm Cúm A cho đến bệnh nghiêm trọng như Ung Thư
+ Chi trả cả các bệnh liên quan đến ThoáiHoáXương
+Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Chi trả khi nằm viện đủ 12 tiếng trở lên  rất nhiều hãng yêu cầu 24 tiếng
+ Thời gian chờ bệnh Đặc Biệt chỉ 90 ngày  nhiều hãng là 365 ngày
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần
+điều trị
+ Bảo vệ tới 75 tuổi dài hạn nhất thị trường BHNT
+ Bảo lãnh các Bệnh Viện Quốc Tế 5 VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN 108
+ Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm Mr Trọng 0987959262 Tư vấn Nhiệt Tình Tận Tâm vì Khách Hàng</t>
         </is>
       </c>
     </row>
@@ -645,11 +687,18 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hoa Dollinda****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Hà Ngọc Mai****Thẻ bảo lãnh 100 viện phí 
+Cho tất cả các thành viên trong gia đình
+ Thanh toán 100 từ viện công cho đến Quốc Tế
+ Ngon bổ rẻ với các bé từ 05 tuổi giá chỉ 2tr1 năm
+ Có thể tham gia rời hoặc kèn HĐ BHNT
+ Cắt thắng lưỡi  các bệnh viêm phổi nạo VA k bị loại trừ liên kết trực tiếp với khoa S bv Nhi Trung Ương
+ Các bệnh xương khớp người già vẫn được thanh toán
+Mn quan tâm ib e tư vấn ạ</t>
         </is>
       </c>
     </row>
@@ -658,11 +707,11 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Mk từng đốt rồi bạn nên mk thấy đốt cũng được bạn tìm chỗ uy tín mà đốt là ko sợ đâu</t>
+          <t>Minh Trang****M cũng ko đánh giá đội ngũ y tá của HN cao ko thể so sánh với Nhi TW Nhưng đúng là nếu bé sốt cao như vậy thì sẽ hơi khó lấy ven đấy mẹ ạ Thường bên nhi TW khoa quốc tế với các bạn sốt cao sẽ được ưu tiên cho uống thuốc hạ sốt trước trong lúc chờ khám</t>
         </is>
       </c>
     </row>
@@ -671,11 +720,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Mã Nam****tình trạng ntn rồi b</t>
+          <t>Hà Ngọc Mai****Em Mai Daiichi muon gui toi cac Mom chuong trinh nhu sau
+ Chuong Trinh Thẻ chăm sóc sức khỏe  du phong thanh toán 100 vien phi tu cong đen quoc te như Vinmec Hồng Ngọc dịch vụ y tế tốt nhất chu đáo nằm phòng 11 tha hồ yên tĩnh nghỉ ngơi Hỗ trợ tiền giường 3 triệungày Chi trả 1 tỷbệnh không giới hạn số bệnh Hỗ trợ tiền giường người thân chăm sóc bé 1 triệungày Cắt thắng lưỡi  các bệnh viêm phổi nạo VA k bị loại trừ liên kết trực tiếp với bv Nhi Trung Ương
+Cac Mom qtam ib e nhe a</t>
         </is>
       </c>
     </row>
@@ -684,11 +735,11 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Hoa Dollinda****Cái nào cug dkmiễn là tìm đúng nơi đúng chỗ nha b</t>
+          <t>Phương Thảo****Ui cái đầu chuẩn luôn b ơi Bé nhà m bị sốt đợt đầu năm tới lấy máu làm xét nghiệm mà các cô loay hoay cả 45 k lấy đc cho con Làm khóc lạc cả giọng</t>
         </is>
       </c>
     </row>
@@ -697,11 +748,11 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Mã Nam****B bị bao lâu rồi</t>
+          <t>Khủng Long****Bé sốt cao thì rất khó lấy ven bé mà gồng lên nữa thì lại càng khó  Nhà t cũng vào đây rất nhiều lần rồi và yêu cầu điều dưỡng từ trên khoa nhi xuống lấy ven  Bh bố mẹ cho con đi viện cũng phải trang bị thêm kiến thức cho mình nữa thì mới đòi quyền lợi cho con dc đấy</t>
         </is>
       </c>
     </row>
@@ -710,11 +761,12 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Nam Carter****nên đi khám đi nhé</t>
+          <t>Phạm Minh Phượng****Thương bé quá Nhỏ xíu nữa chứ  Bạch cầu tiểu cầu giảm như này là sốt xuất huyết à b
+2 tuần trước bé nhà mình 1h đêm đi viện cũng xng máu sốt cao bé nhà mình bthg uống hạ sốt nó vã mồ hôi ra ngay lần này thì ko sốt cao ko hạ cũng xin đc nhập viện nhưng bv quá tải cảm giác bs hơi hời hợt họ ko kết luận dc gì nhiều nên lại đi viện khác chứ chưa điều trị Hồng ngọc</t>
         </is>
       </c>
     </row>
@@ -723,11 +775,11 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Đặng Johnny****B đến pk 120 hoàng quốc việt ở hà nội nhé một lần là khỏi hết đấy</t>
+          <t>Tâm Tâm Nguyễn****Lấy máu kém chuyên nghiệp có tiếng r chị ạ nhiều người kêu lắm</t>
         </is>
       </c>
     </row>
@@ -736,11 +788,11 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Nam Carter****</t>
+          <t xml:space="preserve">Thuỳ Nguyễn****Con mình cũng như thế lấy máu 45 lần không được thì đổ lỗi do con to nên không thấy ven con khoẻ dãy quá không trọc đúng ven </t>
         </is>
       </c>
     </row>
@@ -749,11 +801,11 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Phan Thanh Hằng****đốt cho nhanh khỏi em nhé</t>
+          <t>Hà Lê****Đúng thật con sốt mệt mà cảnh đi chờ đợi khám 5 tiếng nghĩ khổ ghê</t>
         </is>
       </c>
     </row>
@@ -762,11 +814,11 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Khoa Hòa Hiệp****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Nguyễn Quang Huy****Trong tình trạng các viện nhi đều quá tải thì phải chấp nhận thôi Dịch vụ nthe cũng ok hơn so với vào nhi quốc tế r b</t>
         </is>
       </c>
     </row>
@@ -775,11 +827,24 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Mk theo bs Trang pshn đốt lúc đang đốt cũng hơi đau tí nhưng được cái đốt xong bs tư vấn nhiệt tình về cách vệ sinh h khỏi rồi và mk đang bầu nữa</t>
+          <t>Phạm Oanh****Chỉ với 21 triệunăm phí trẻ nhỏ Bảo Hiểm chi trả viện phí 1 TỶ ĐỒNG1 BỆNH
+ Tien phong va an uong 3 triệungay
+Tiền giường cho người thân 1trngày
+ Phẫu thuật 75 triệuca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệuca
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản Khuyết Tật Bẩm Sinh
+ Chi trả cả các bệnh liên quan đến Thoái Hoá Xương Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần điều trị
+ Bảo lãnh các Bệnh Viện Quốc Tế 5  VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN TÂM ANH HỒNG NGỌC
+Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm PHẠM OANH DAIICHI 0977077808 Tư vấn Nhiệt Tình Tận Tâm vì khách hàng</t>
         </is>
       </c>
     </row>
@@ -788,11 +853,11 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Khoa Hòa Hiệp****B bị bao lâu rồi</t>
+          <t>Vân Ngô****Công nhận Dịch vụ khám ở Hồng Ngọc kém chuyên nghiệp Đẻ thì không biết thế nào</t>
         </is>
       </c>
     </row>
@@ -801,11 +866,12 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hi Thiện Nhân****Thực ra ở ctc nó không nhiều dây thần kinh cảm giác vậy đâu em chỉ hơi tức thốn tí thôi Em vlt độ 3 có thể đốt hoặc phun lạnh đều được em nhé Đừng lo</t>
+          <t>Phương Ngọc****mom oi bên Daiichi đang có thẻ CSSK cho bé từ 30 ngày tuỏi trở lên Đi khám hay nằm viện thì tấm thẻ CSSK này sẽ thanh toán 80100 chi phí viện phí tại tất cả các bệnh viện trên cả nước từ các bênh viện công tư cho tới các bệnh viện quốc tế Thủ tục thanh toán siêu nhanh siêu đơn giản các mom chỉ cần đưa con vào thẳng bệnh viên mà ko cần phải chờ đợi con ko bị lây chéo ai nhất là trong mùa dịch bệnh nguy hiểm này  Mom quan tâm ib để em có cơ hội để giúp đỡ ạ
+Lh 0969783880</t>
         </is>
       </c>
     </row>
@@ -814,11 +880,11 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Đào Mỹ Dung****tình trạng ntn rồi b</t>
+          <t>Hà Huyền****Hôm mình cho con đi khám cũng làm xn y như b nhg bs chỉ định luôn xn 5 thứ cùng lúc nên nhanh gọn lấy mẫu 1 lần và chờ khoảng 40 là thấy gọi xg có kết qả r</t>
         </is>
       </c>
     </row>
@@ -827,11 +893,11 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Đào Mỹ Dung****</t>
+          <t xml:space="preserve">Bích Phương****Phúc An Lễ  Mâm Cúng Đầy Tháng Thôi Nôi Trọn Gói Hà Nội Mời Mom tham khảo dịch vụ Mâm Lễ cúng Đầy Tháng Thôi Nôi cho bé nhà mình ạ </t>
         </is>
       </c>
     </row>
@@ -840,11 +906,11 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Phan Thanh Hằng****nên đi khám đi nhé</t>
+          <t>Thực Phẩm Sạch HG****hic sợ</t>
         </is>
       </c>
     </row>
@@ -853,11 +919,11 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Khoa Hòa Hiệp****Em đến pk 120 hoàng quốc việt nhé ok lắm  nếu em là sv còn đc giảm nữa đấy</t>
+          <t>Cẩm Tú Bùi****Hic</t>
         </is>
       </c>
     </row>
@@ -866,11 +932,11 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Phan Thanh Hằng****E đến PK 120 hoàng quốc việt bs Nhạ pshn nhé</t>
+          <t>Minh Dương****Sốt có cho hạ sốt trước k ạ M thì k nhẫn nhink dc như bme bên đó</t>
         </is>
       </c>
     </row>
@@ -879,11 +945,14 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Khoa Hòa Hiệp****nên đi khám đi nhé</t>
+          <t>Lê Bích Thủy****Tham gia tìm hiểu và sẻ chia cùng chúng tôi https
+wwwfacebookcom
+groups
+baohiemdaiichi</t>
         </is>
       </c>
     </row>
@@ -892,11 +961,30 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Mk cũng bị độ 2 theo khám ở pk sản phụ khoa Thắng Trang 208 Nguyễn Ngọc Nại quận Thanh Xuân bạn</t>
+          <t>Bảo Hiểm Dai-ichi**** Chỉ với 21 triệunăm phí trẻ nhỏ Bảo Hiểm chi trả viện phí 1 TỶ ĐỒNG1 BỆNH  không cần kèm bố mẹ  phí rẻ nhất các công ty BHNT
+ Bạn quan tâm bảo vệ sức khỏe Gia Đình hãy tham khảo gói BHNT Daiichi  Thẻ Chăm Sóc Sức Khỏe Tỷ suất sinh lời từ 1317năm trung bình trả 5 năm gần đây
+ Bảo vệ cả gia đình trên 1 hợp đồng
+ Tien phong va an uong 3000000ngay
+ Phẫu thuật 75trca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệuca
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản Khuyết Tật Bẩm Sinh
+ Chi trả cho các bệnh từ nhẹ như Cảm Cúm Cúm A cho đến bệnh nghiêm trọng như Ung Thư
+ Chi trả cả các bệnh liên quan đến Thoái Hoá Xương Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Chi trả khi nằm viện đủ 12 tiếng trở lên  rất nhiều hãng yêu cầu 24 tiếng
+ Thời gian chờ bệnh Đặc Biệt chỉ 90 ngày  nhiều hãng là 365 ngày
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần
+điều trị
+ Bảo vệ tới 75 tuổi dài hạn nhất thị trường BHNT
+ Bảo lãnh các Bệnh Viện Quốc Tế 5 VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN 108
+ Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm Mr Trọng 0987959262 Tư vấn Nhiệt Tình Tận Tâm vì khách hàng</t>
         </is>
       </c>
     </row>
@@ -905,11 +993,11 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Đào Mỹ Dung****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Nguyễn Thu Thủy****Bv hnay có đông lắm k m Cùng ngành đáng ra p bênh nhau nhưng mà chỗ xn kia 30p thôi cho cả tgian chờ các bn khác là 1 tiếng ý Khổ thân thằng chó con</t>
         </is>
       </c>
     </row>
@@ -918,11 +1006,11 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Minh Anh****B độ mấy r Nếu độ 3 thì mới nên đốt Mà mình thấy bên pkham bsi trang pshn đốt hết có 34tr thoi</t>
+          <t>Nguyễn Thị Hoài****Sú sôt hả con</t>
         </is>
       </c>
     </row>
@@ -931,11 +1019,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Trang Nguyen****Tốt nhất vào phụ sản trung ương e nh</t>
+          <t>Hà Ngọc Mai****Em Mai Daiichi muon gui toi cac Mom chuong trinh nhu sau
+ Chuong Trinh Thẻ chăm sóc sức khỏe  du phong thanh toán 100 vien phi tu cong đen quoc te như Vinmec Hồng Ngọc dịch vụ y tế tốt nhất chu đáo nằm phòng 11 tha hồ yên tĩnh nghỉ ngơi Hỗ trợ tiền giường 3 triệungày Chi trả 1 tỷbệnh không giới hạn số bệnh Hỗ trợ tiền giường người thân chăm sóc bé 1 triệungày Cắt thắng lưỡi  các bệnh viêm phổi nạo VA k bị loại trừ liên kết trực tiếp với bv Nhi Trung Ương
+Cac Mom qtam ib e nhe a</t>
         </is>
       </c>
     </row>
@@ -944,11 +1034,24 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cát Mộng Liễu****tình trạng ntn rồi b</t>
+          <t>Phạm Oanh****all Chỉ với 21 triệunăm phí trẻ nhỏ Bảo Hiểm chi trả viện phí 1 TỶ ĐỒNG1 BỆNH
+ Tien phong va an uong 3 triệungay
+Tiền giường cho người thân 1trngày
+ Phẫu thuật 75 triệuca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệuca
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản Khuyết Tật Bẩm Sinh
+ Chi trả cả các bệnh liên quan đến Thoái Hoá Xương Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần điều trị
+ Bảo lãnh các Bệnh Viện Quốc Tế 5  VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN TÂM ANH HỒNG NGỌC
+Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm PHẠM OANH DAIICHI 0977077808 Tư vấn Nhiệt Tình Tận Tâm vì khách hàng</t>
         </is>
       </c>
     </row>
@@ -957,11 +1060,11 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Đào Mỹ Dung****B bị bao lâu rồi</t>
+          <t>Hong Nhung****Hung Ca</t>
         </is>
       </c>
     </row>
@@ -970,11 +1073,11 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Cát Mộng Liễu****</t>
+          <t>Ajarn Andy****hôm trc nhà mình đi khám cũng vậy bảng thi hiện đến lượt mà mãi chả thấy gọi Hỏi thì cứ chờ chút xíu Đến lúc gắt lên thì mời vào rồi giải thích lý do abcz Max mệt luôn</t>
         </is>
       </c>
     </row>
@@ -983,11 +1086,11 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Đào Ngọc Ngân****Qtam ạ</t>
+          <t>Lại Diệu Linh****Tư vấn ạ</t>
         </is>
       </c>
     </row>
@@ -996,11 +1099,11 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Phòng Khám Phụ Khoa****ib chị tư vấn</t>
+          <t>Quý Tồ****Đính kèm bảo hiểm nhân thọ ko b</t>
         </is>
       </c>
     </row>
@@ -1009,11 +1112,11 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Vẫn có bé được mom trc mk bị độ 2 theo đốt chỗ bs Trang h đang có bé đây</t>
+          <t>Ngọc Thu****Ib ạ</t>
         </is>
       </c>
     </row>
@@ -1022,11 +1125,11 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Minh Anh****Đốt dc b nha k sao Mình cx đốt bên bsi trang pshn h vẫn có bé bth đây</t>
+          <t>Thanh Nga****chị chekc ib em nhé</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1142,28 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Mã Nam****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Bảo Hiểm Dai-ichi**** Bảo Hiểm DAIICHI chi trả viện phí lên tới 1 TỶ ĐỒNG1 BỆNH
+ Bạn quan tâm bảo vệ sức khỏe Gia Đình hãy tham khảo gói BHNT Daiichi  Thẻ Chăm Sóc Sức Khỏe Tỷ suất sinh lời từ 1317năm trung bình trả 5 năm gần đây
+ Phí thẻ trẻ nhỏ rẻ chỉ từ 21 triệu năm
+ Tien phong va an uong 3000000ngay
+ Phẫu thuật 75trca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệu
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản KhuyếtTậtBẩm
+Sinh
+ Chi trả cho các bệnh từ nhẹ như Cảm Cúm Cúm A cho đến bệnh nghiêm trọng như Ung Thư
+ Chi trả cả các bệnh liên quan đến ThoáiHoáXương
+Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Chi trả khi nằm viện đủ 12 tiếng trở lên  rất nhiều hãng yêu cầu 24 tiếng
+ Thời gian chờ bệnh Đặc Biệt chỉ 90 ngày  nhiều hãng là 365 ngày
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần
+điều trị
+ Bảo vệ tới 75 tuổi dài hạn nhất thị trường BHNT
+ Bảo lãnh các Bệnh Viện Quốc Tế 5 VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN 108
+ Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm Mr Trọng 0987959262 Tư vấn Nhiệt Tình Tận Tâm vì Khách Hàng</t>
         </is>
       </c>
     </row>
@@ -1052,7 +1176,10 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mã Nam****E mới đốt 18 ngày ckk đến trk 4 ngày và máu ra nhiều lắm còn phải ut cầm máu đó</t>
+          <t>Đặng Bích Ngọc****tham gia chia sẻ và tìm hiểu sản phẩm nhất định nên mua cho cả mẹ và bé https
+wwwfacebookcom
+groups
+baohiemdaiichi</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1192,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Hoa Dollinda****Chu kì ngay sau đốt thì thường sẽ kéo dài nhiều ngày lượng cũng nhiều em ạ</t>
+          <t>Phương Trần****Chấm chấm</t>
         </is>
       </c>
     </row>
@@ -1078,7 +1205,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Minh Uyên Tinh****nên đi khám đi nhé</t>
+          <t>Thanh Nga****</t>
         </is>
       </c>
     </row>
@@ -1087,11 +1214,11 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Nam Carter****B bị bao lâu rồi</t>
+          <t>Liên Luật Bảo Hiểm****Thẻ bhyt và thẻ bảo lãnh khi sử dụng gói sinh tại Hồng Ngọc  PTM các Mon tham khảo nhea</t>
         </is>
       </c>
     </row>
@@ -1100,11 +1227,11 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Nam Carter****tình trạng ntn rồi b</t>
+          <t>Tom Tom****Như thế nào vậy ạ</t>
         </is>
       </c>
     </row>
@@ -1113,11 +1240,12 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Minh Uyên Tinh****</t>
+          <t>Phương Ngọc****mom oi bên Daiichi đang có thẻ CSSK cho bé từ 30 ngày tuỏi trở lên Đi khám hay nằm viện thì tấm thẻ CSSK này sẽ thanh toán 80100 chi phí viện phí tại tất cả các bệnh viện trên cả nước từ các bênh viện công tư cho tới các bệnh viện quốc tế Thủ tục thanh toán siêu nhanh siêu đơn giản các mom chỉ cần đưa con vào thẳng bệnh viên mà ko cần phải chờ đợi con ko bị lây chéo ai nhất là trong mùa dịch bệnh nguy hiểm này  Mom quan tâm ib để em có cơ hội để giúp đỡ ạ
+Lh 0969783880</t>
         </is>
       </c>
     </row>
@@ -1126,11 +1254,11 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Huỳnh Thanh Việt Nga****Dùng bột nhội hiệu quả lm c ạ chứ e cx đi khám bsi toàn đặt ksinh khỏi lại bị lại chán lm mà tiền thuốc phụ khoa mắc kinhhh </t>
+          <t>Hằng Nguyễn****Cho mình xin thông tin với ạ</t>
         </is>
       </c>
     </row>
@@ -1139,11 +1267,11 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Hoà Khánh****Viêm này điều trị dai dẳng lắm mình điều trị kết hợp với dùng phòng ngừa tái lại bằng hyalosan bổ sung lợi khuẩn mới ổn được đóbạn vào đây Hyalosan Yêu Thương Phái Đẹp nhờ chị ds tv cho</t>
+          <t>Kiều Linh****Làm đc ở bv thể thao việt nam ko b</t>
         </is>
       </c>
     </row>
@@ -1152,11 +1280,11 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Lê Văn Sơn****Lần gần nhất bạn đi khám phụ khoa là khi nào Đã làm những xét nghiệm gì và kết quả ra sao nè</t>
+          <t>Dương Thị Lệ****Ib minh</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1297,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Phạm Mai Hoa****Bạn đi khám và đặt thuốc theo chỉ định của bác sĩ thôi</t>
+          <t>Vân Vân****Ib tư vấn t vs ak</t>
         </is>
       </c>
     </row>
@@ -1182,7 +1310,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Trần Anh Huy****B bị bao lâu rồi</t>
+          <t>Phạm Oanh****e qt ạ</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1323,13 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Ly Ly****nên đi khám đi nhé</t>
+          <t>Phạm Oanh****Chỉ với 21 triệunăm phí trẻ nhỏ Bảo Hiểm chi trả viện phí 1 TỶ ĐỒNG1 BỆNH
+ Tien phong va an uong 3 triệungay
+Tiền giường cho người thân 1trngày
+ Phẫu thuật 75 triệuca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệuca
+ Chi phi xe cứu thư</t>
         </is>
       </c>
     </row>
@@ -1208,7 +1342,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Ly Ly****tình trạng ntn rồi b</t>
+          <t>Hương Quỳnh****Ib e vs ạ</t>
         </is>
       </c>
     </row>
@@ -1221,8 +1355,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Lam Tat Hieu****Trước c cũng bầu lúc đang vlt toàn bộ ctc e ạ Gần như dùng bvs suốt luôn
-E rửa nước là chè lá trầu nhiều nó thâm sỉn vùng kín lắm chưa kể lại ảnh hưởng pH âm đạo</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1235,7 +1368,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Phương Linh Hà****Nói chứ mỗi lần đi bv khám cực khổ lắm ấy Bốc số đợi chờ mãi đến lượt vào bác sĩ khám qua loa chưa được 5p là xong May mình biết đến nhà thuốc này Hyalosan Yêu Thương Phái Đẹp Hàng Châu Âu được Bộ Y tế Việt Nam cấp phép trang thiết bị y tế dùng cũng yên tâm Mỗi lần mình có thắc mắc gì hỏi bên này được hỗ trợ tư vấn nhiệt tình cẩn thận lắm</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1381,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Lam Tat Hieu****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1394,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Hoà Khánh****Viêm này điều trị dai dẳng lắm mình điều trị kết hợp với dùng phòng ngừa tái lại bằng hyalosan bổ sung lợi khuẩn mới ổn được đóbạn vào đây Hyalosan Yêu Thương Phái Đẹp nhờ chị ds tv cho</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1407,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Trần Anh Huy****</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1283,11 +1416,15 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Trần Anh Huy****Li ti thì kphai em ạ Herpes mụn rộp sinh dục nó sẽ như nốt thuỷ đậu ý khi cbi phát bệnh thì em sẽ thấy đau nhức vùng kín nốt mọc lên sẽ gây đau rát vì lở loét khi vỡ hết thì nó mọc da non gây ngứa ngáy</t>
+          <t>Hồ Mai Ngọc****các mom ơi vào đây xem nhiều mẹ chia sẻ kinh nghiệm bầu bí chọn sữa chăm con easy hay lắm nuôi con nhàn tênh https
+wwwfacebookcom
+groups
+3399014686990329
+refshare</t>
         </is>
       </c>
     </row>
@@ -1296,11 +1433,11 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Trần Anh Huy****Mng ai biết chỉ mình nữa với ạ</t>
+          <t>Hiền Đặng****Ib m nha</t>
         </is>
       </c>
     </row>
@@ -1309,11 +1446,11 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Lam Tat Hieu****C nghĩ do ẩm ướt nhiều nên nó vậy thôi E nghi ngờ thì tốt nhất đi khám bác cho thuốc bôi sẽ nhanh đỡ hơn</t>
+          <t>Ánh Dương****Ib mình</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1463,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Phương Linh Hà****Nói chứ mỗi lần đi bv khám cực khổ lắm ấy Bốc số đợi chờ mãi đến lượt vào bác sĩ khám qua loa chưa được 5p là xong May mình biết đến nhà thuốc này Hyalosan Yêu Thương Phái Đẹp Hàng Châu Âu được Bộ Y tế Việt Nam cấp phép trang thiết bị y tế dùng cũng yên tâm Mỗi lần mình có thắc mắc gì hỏi bên này được hỗ trợ tư vấn nhiệt tình cẩn thận lắm</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1476,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Hoà Khánh****Viêm này điều trị dai dẳng lắm mình điều trị kết hợp với dùng phòng ngừa tái lại bằng hyalosan bổ sung lợi khuẩn mới ổn được đóbạn vào đây Hyalosan Yêu Thương Phái Đẹp nhờ chị ds tv cho</t>
+          <t>Liên Luật Bảo Hiểm****</t>
         </is>
       </c>
     </row>
@@ -1348,11 +1485,11 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Phong Trần****nên đi khám đi nhé</t>
+          <t>Liên Luật Bảo Hiểm****</t>
         </is>
       </c>
     </row>
@@ -1361,11 +1498,11 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Ly Ly****B bị bao lâu rồi</t>
+          <t>Liên Luật Bảo Hiểm****Liên Luật Bảo Hiểm</t>
         </is>
       </c>
     </row>
@@ -1374,11 +1511,11 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Ly Ly****tình trạng ntn rồi b</t>
+          <t>向日葵****Cho m hỏi chút ạm o phòng đôi hay đơn đấy ạphí ntn ạ</t>
         </is>
       </c>
     </row>
@@ -1387,11 +1524,11 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Phong Trần****</t>
+          <t>Hải Yến****Mẹ nó dùng thẻ BH của bên nào đó ạ</t>
         </is>
       </c>
     </row>
@@ -1400,13 +1537,32 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Lê Thị Thu Hiên****e xem qua video nhé https
-youtube
-kAbmSV87UE</t>
+          <t>Bảo Hiểm Dai-ichi**** Bao Hiem DAIICHI chi tra vien phi len toi 1 TY ĐONG1 BENH
+ Ban quan tam bao ve suc khoe Gia Đinh hay tham khao goi BHNT Daiichi  The Cham Soc Suc Khoe Ty suat sinh loi tu 1317nam trung binh tra 5 nam gan đay
+ Phi tre nho re chi tu 21 trieu nam phi re nhat cac cong ty BHNT
+ Tien phong va an uong 3000000ngay
+ Phau thuat 75trca
+ Phong cham soc Đac Biet 5250000ngay
+ Cay ghep bo phan 500 trieuca
+ Chi phi xe cuu thuong 100
+ Đieu tri ung thu  100
+ Chi tra cho ca cac Bien Chung Thai San KhuyetTat
+BamSinh
+ Chi tra cho cac benh tu nhe nhu Cam Cum Cum A cho đen benh nghiem trong nhu Ung Thu
+ Chi tra ca cac benh lien quan đen ThoaiHoaXu
+ongKhop Loang Xuong Thoat Vi Đia Đem
+ Chi tra khi nam vien đu 12 tieng tro len  rat nhieu hang yeu cau 24 tieng
+ Thoi gian cho benh Đac Biet chi 90 ngay  nhieu hang la 365 ngay
+ Khong gioi han so lan nam vien va thoi gian cho giua cac lan
+đieu tri
+ Bao ve toi 75 tuoi dai han nhat thi truong BHNT
+ Bao lanh cac Benh Vien Quoc Te 5 VINMEC VIET PHAP VIET ĐUC NHI TW VIEN 108
+ Inbox cho minh đe đuoc tu van chi tiet nhieu quyen loi khac nua
+Truong nhom Mr Trong 0987959262 Tu van Nhiet Tinh Tan Tam vi Khach Hang</t>
         </is>
       </c>
     </row>
@@ -1415,11 +1571,11 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Hoà Khánh****Viêm này điều trị dai dẳng lắm mình điều trị kết hợp với dùng phòng ngừa tái lại bằng hyalosan bổ sung lợi khuẩn mới ổn được đóbạn vào đây Hyalosan Yêu Thương Phái Đẹp nhờ chị ds tv cho</t>
+          <t>Nguyen Vu Hung****vô đây hỏi mom ạ  nhiều mom chia sẻ kiến thức chăm con nhỏ hay lắm nuôi con không kháng sinh Mẹ Thông Thái Nuôi Con Khoa Học</t>
         </is>
       </c>
     </row>
@@ -1428,11 +1584,15 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Lê Thị Thu Hiên****add zalo bsi để được tư vấn kỹ hơn 0966688152</t>
+          <t>Anh Khoa Võ****các mom ơi vào đây xem nhiều mẹ chia sẻ kinh nghiệm bầu bí chọn sữa chăm con easy hay lắm nuôi con nhàn tênh https
+wwwfacebookcom
+groups
+3399014686990329
+refshare</t>
         </is>
       </c>
     </row>
@@ -1441,11 +1601,11 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Trc mk cũng bị viêm mà nhẹ hơn bạn chút mk khám chỗ bs Trang pshn Bs nhiệt tình nhẹ nhàng lắm</t>
+          <t>Bống Nhí Nhố****Ib mình với ạ</t>
         </is>
       </c>
     </row>
@@ -1454,11 +1614,11 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Hoàng Nguyệt****Bạn muốn vào viện thì đi viện pshn mà viện thì thường hay đông lắm Trc mk cũng đi khám ở viện mấy lần bị đợi lâu nên h toàn đi phòng khám của bs Trang khám thôi bác là bs pshn luôn</t>
+          <t>Quỳnh Quỳnh****Ib ạ</t>
         </is>
       </c>
     </row>
@@ -1467,11 +1627,11 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Trần Anh Huy****Phụ sản hà nội thì sẽ đỡ đông hơn pstw e nhé Chi phí khám 2 nơi tương đương nhau e nên đi sớm để có thể làm đầy đủ các bước thăm khám đợi kq trong 1 buổi e ạ</t>
+          <t>Khúc Hồng Ngọc****Ib m</t>
         </is>
       </c>
     </row>
@@ -1480,11 +1640,11 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Ly Ly****Em muốn vào viện thì cứ vảo phụ sản trung ương hoặc psan hanoi nha</t>
+          <t>Nhung Nguyễn****ib m</t>
         </is>
       </c>
     </row>
@@ -1493,11 +1653,15 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Phong Trần****Em khám cho cả ny nữa nha và chờ kqua xem sao Lậu sẽ có xn riêng đó em Chú ý đi nhà nghỉ hoặc csong hàng ngày đừng dùng chung đồ chung khăn vs ai em nhé c gặp rất nhiều ng vậy rồi nguồn lây kphai do ck không do mình nhưng vẫn bệnh là vậy đó</t>
+          <t>Xavia Trần****Các bác nào muốn hỏi về thuốc mà muốn bác sĩ với dược sĩ trả lời thì ib Page này nè https
+wwwfacebookcom
+hoidapthuocvietn
+am
+Ib trả lời ngay mà còn tư vấn miễn phí</t>
         </is>
       </c>
     </row>
@@ -1506,11 +1670,11 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Ly Ly****Trước tiên thì e đợi kết quả xng Nếu đúng là e bị thì bạn ny cũng cần đi khám e nhé cái này có thể e lây từ ny e hoặc  nhỏ là dùng chung đồ  khăn tắm quần với ng có bệnh Chữa có thể khỏi e nha e đừng lo lắng quá bình tĩnh đợi thêm xem sao đã</t>
+          <t>Ngô Duy Bằng****vô đây hỏi mom ạ  nhiều mom chia sẻ kiến thức chăm con nhỏ hay lắm nuôi con không kháng sinh Mẹ Thông Thái Nuôi Con Khoa Học</t>
         </is>
       </c>
     </row>
@@ -1519,11 +1683,11 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hoa****Mk đốt ở pk tư của bác sĩ Trang chi phí cũng hợp lý thôi bạn cũng không mất quá nhiều linh tinh đâu Và đốt xong mk vẫn mang bầu bình thường được</t>
+          <t>Ốc Hiền****Ib m nhé</t>
         </is>
       </c>
     </row>
@@ -1532,13 +1696,11 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Phạm Mai Hoa****Pp RFA thực tế k cần thiết để đtri vlt đâu e Nó tốn kém và ít nơi làm pp đó lắm
-Thay vào đó e chọn đốt leep đều ok rồi nhé
-C cũng vlt diện rộng đã đốt và khỏi rồi nè</t>
+          <t>Hải Yến****Em đang ctrinh tặng thẻ CSSK Daiichi cho bé mẹ nào qtam em gửi tham khảo ạ</t>
         </is>
       </c>
     </row>
@@ -1547,12 +1709,11 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Lê Văn Sơn****B qua bác nhạ 120 hoàng quốc việt hn
-Mình cũng lộ tuyến chưa khỏi 1 năm nay đang có e bé r nè</t>
+          <t>Kim Dung****Ít lắm b Con mình nằm viện hết 36tr nhg BHYT chỉ thanh toán 2tr thôi</t>
         </is>
       </c>
     </row>
@@ -1561,11 +1722,11 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Trieu Tu Huy****Không ảnh hưởng j đâu em Nếu em không có khó chịu j thì kệ nó cũng ksao Xn tầm soát utctc định kì là đc</t>
+          <t>Hải Yến****ít lắm c ơi có ddkien c mua BHNT bảo vệ cho bố mẹ E đang có thẻ cssk cao cấp tặng bé 1 năm đầu đi viện chi trả gần hết cho con c nhé</t>
         </is>
       </c>
     </row>
@@ -1574,11 +1735,11 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Lê Văn Sơn****tình trạng ntn rồi b</t>
+          <t>Bảo Hiểm Dai-ichi****Chỉ được một vài danh mục của BHYT thôi bạn không đáng bao nhiêu đâu Tiền giường chắc chắn không được rồi</t>
         </is>
       </c>
     </row>
@@ -1587,11 +1748,11 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Huỳnh Thanh Việt Nga****B bị bao lâu rồi</t>
+          <t>Phạm Hồng Ngọc****Nhưng mẹ cháy túi hahâ</t>
         </is>
       </c>
     </row>
@@ -1600,11 +1761,11 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Hoà Khánh****Viêm này điều trị dai dẳng lắm mình điều trị kết hợp với dùng phòng ngừa tái lại bằng hyalosan bổ sung lợi khuẩn mới ổn được đóbạn vào đây Hyalosan Yêu Thương Phái Đẹp nhờ chị ds tv cho</t>
+          <t>Hải Yến****Công nhận HN ytam cả về chất lượng Dv và Y bác sĩ các c ạ Bên cty Daiichi e đang có ctrinh tặng thẻ Cssk cao cấp cho bé 1 năm Mẹ nào cần ib em nha</t>
         </is>
       </c>
     </row>
@@ -1613,11 +1774,11 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Huỳnh Thanh Việt Nga****nên đi khám đi nhé</t>
+          <t>Minh Dương****Chúc mừng con</t>
         </is>
       </c>
     </row>
@@ -1626,266 +1787,32 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Ton Thanh Viet****Mng ai biết chỉ mình nữa với ạ</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="n">
-        <v>17</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Ton Thanh Viet****Bạn uống men vi sinh otipac đi mình thấy ok lắmmình uống mình thấy đỡ ý</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="n">
-        <v>17</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Lê Thị Thu Hiên****Không cần đốt cũng chữa khỏi vlt ctc nhé e https
-youtube
-oQimf8XAHTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="n">
-        <v>17</v>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Lê Văn Sơn****</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="n">
-        <v>18</v>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Mã Nam****Mình độ 2 Và còn chửa đẻ thêm nên mình cũng chưa đốt Bà mình làm bên bác sĩ nói giờ đi đâu cũng nói đốt  nhưng đốt có người vẫn tái lại bà mình bảo độ 3 cũng k đốt trừ khi rất nặng mới đốt</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="n">
-        <v>18</v>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Lê Thị Thu Hiên****k cần đốt nhé e https
-youtube
-oQimf8XAHTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="n">
-        <v>18</v>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Minh Uyên Tinh****Mng ai biết chỉ mình nữa với ạ</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="n">
-        <v>18</v>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Hoa Dollinda****C đây vẫn để nguyên Bổ sung định kì vtmE vs vệ sinh thui nên nó không rộng ra và không gây khó chịu j 4 năm rồi vẫn đẻ bt</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="n">
-        <v>18</v>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Xavia Trần****Bác muốn hỏi về bệnh thuốc hay thực phẩm chức năng thì hỏi bên này nè https
-wwwfacebookcom
-hoidapthuocvietn
-am
-Toàn các bác sĩ và dược sĩ tư vấn cho thôi còn không mất phí</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="n">
-        <v>18</v>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Nam Carter****tình trạng ntn rồi b</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="n">
-        <v>18</v>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Huyền Diệu****B bị độ mấy rồi viêm lt nếu ko tìm nơi uy tín để đốt thì cứ tái đi tái lại rất khó chịu luôn</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="n">
-        <v>18</v>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Minh Uyên Tinh****</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="n">
-        <v>18</v>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Mã Nam****B bị bao lâu rồi</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="n">
-        <v>18</v>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Nam Carter****nên đi khám đi nhé</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="n">
-        <v>19</v>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Lam Tat Hieu****B bị bao lâu rồi</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="n">
-        <v>19</v>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Phạm Mai Hoa****Mng ai biết chỉ mình nữa với ạ</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="n">
-        <v>19</v>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Phạm Mai Hoa****C đã uống và nó làm men gan cao e nhé Nên cân nhắc kĩ vì giá nó cũng khá chát theo được nó thì cũng cả vấn đề đó e ạ</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="n">
-        <v>19</v>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Trần Anh Huy****tình trạng ntn rồi b</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="n">
-        <v>19</v>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Trần Anh Huy****nên đi khám đi nhé</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="n">
-        <v>19</v>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Lam Tat Hieu****Thấy phí tiền ạ K khỏi dc bệnh mà còn mắc nữa Hoặc do cơ địa k phù hợp ạ</t>
+          <t>Bảo Hiểm Dai-ichi**** Bảo Hiểm DAIICHI chi trả viện phí lên tới 1 TỶ ĐỒNG1 BỆNH
+ Bạn quan tâm bảo vệ sức khỏe Gia Đình hãy tham khảo gói BHNT Daiichi  Thẻ Chăm Sóc Sức Khỏe Tỷ suất sinh lời từ 1317năm trung bình trả 5 năm gần đây
+ Phí thẻ trẻ nhỏ rẻ chỉ từ 21 triệu năm
+ Tien phong va an uong 3000000ngay
+ Phẫu thuật 75trca
+ Phòng cham soc Đac Biet 5250000ngay
+ Cấy ghép bộ phận 500 triệu
+ Chi phi xe cứu thương 100
+ Đieu tri ung thu  100
+ Chi trả cho cả các Biến Chứng Thai Sản KhuyếtTậtBẩm
+Sinh
+ Chi trả cho các bệnh từ nhẹ như Cảm Cúm Cúm A cho đến bệnh nghiêm trọng như Ung Thư
+ Chi trả cả các bệnh liên quan đến ThoáiHoáXương
+Khớp Loãng Xương Thoát Vị Đĩa Đệm
+ Chi trả khi nằm viện đủ 12 tiếng trở lên  rất nhiều hãng yêu cầu 24 tiếng
+ Thời gian chờ bệnh Đặc Biệt chỉ 90 ngày  nhiều hãng là 365 ngày
+ Không giới hạn số lần nằm viện và thời gian chờ giữa các lần
+điều trị
+ Bảo vệ tới 75 tuổi dài hạn nhất thị trường BHNT
+ Bảo lãnh các Bệnh Viện Quốc Tế 5 VINMEC VIỆT PHÁP VIỆT ĐỨC NHI TW VIỆN 108
+ Inbox cho mình để được tư vấn chi tiết nhiều quyền lợi khác nữa
+Trưởng nhóm Mr Trọng 0987959262 Tư vấn Nhiệt Tình Tận Tâm vì Khách Hàng</t>
         </is>
       </c>
     </row>

</xml_diff>